<commit_message>
Added the rest of simple prompt solutions and included google gemini
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paweł Skorupa\Desktop\Magisterskie\masters\AI-tools-assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1999F5B-E452-4E39-9BAC-E9AD027C0FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1D96E4-464D-4AE3-8895-3565BE90BC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{666B9FA9-F2C9-479A-B3E1-10E6830D7CA5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{666B9FA9-F2C9-479A-B3E1-10E6830D7CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="30">
   <si>
     <t>ChatGPT</t>
   </si>
@@ -120,6 +121,12 @@
   </si>
   <si>
     <t>Tabnine</t>
+  </si>
+  <si>
+    <t>Complex</t>
+  </si>
+  <si>
+    <t>DeepSeek</t>
   </si>
 </sst>
 </file>
@@ -539,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE26591-5507-4A9E-8E80-9C468468F115}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,6 +560,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -613,6 +623,9 @@
       <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -636,6 +649,9 @@
       <c r="G4" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H4" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -658,6 +674,9 @@
       </c>
       <c r="G5" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -695,6 +714,9 @@
       <c r="G7" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="H7" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -718,6 +740,9 @@
       <c r="G8" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H8" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -741,6 +766,9 @@
       <c r="G9" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H9" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -764,6 +792,9 @@
       <c r="G10">
         <v>53</v>
       </c>
+      <c r="H10">
+        <v>355</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -786,6 +817,9 @@
       </c>
       <c r="G11">
         <v>377</v>
+      </c>
+      <c r="H11">
+        <v>69792</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -823,6 +857,9 @@
       <c r="G13" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H13" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -846,6 +883,9 @@
       <c r="G14" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H14" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -869,6 +909,9 @@
       <c r="G15" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H15" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -892,6 +935,9 @@
       <c r="G16" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H16" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -913,6 +959,9 @@
         <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -951,6 +1000,9 @@
       <c r="G19" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="H19" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -974,6 +1026,9 @@
       <c r="G20" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H20" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -996,6 +1051,9 @@
       </c>
       <c r="G21" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1033,6 +1091,9 @@
       <c r="G23" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H23" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1056,6 +1117,9 @@
       <c r="G24" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H24" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1079,6 +1143,9 @@
       <c r="G25" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="H25" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -1100,6 +1167,9 @@
         <v>9</v>
       </c>
       <c r="G26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1161,9 +1231,84 @@
       <c r="G29">
         <v>0</v>
       </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD17AC5-5E62-4EC9-9784-97E7492AA189}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>